<commit_message>
boss pattern by server
more parameters added
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/boss_pattern.xlsx
+++ b/Engine/data/datasheet/boss_pattern.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\datasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7342BC0-238D-45E9-A1D6-FBD973DEB757}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36973B1B-A7EF-4849-91FE-1228440CBD51}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="25">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -91,6 +91,34 @@
   </si>
   <si>
     <t>how long will bullets exist</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>straight(0), follow player(1)</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BULLET_SLOW_FRAME</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BULLET_TYPE</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>frame before bullet accelerates</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>BULLET_SPEED</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>float</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1159,10 +1187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1201,309 +1229,429 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="B3" s="5">
-        <v>3</v>
-      </c>
       <c r="C3" s="5" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B5" s="10">
-        <v>200</v>
+        <v>0.7</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>17</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="5">
         <v>3</v>
       </c>
-      <c r="B6" s="5">
-        <v>4</v>
-      </c>
       <c r="C6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="5">
+        <v>10</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="10">
+        <v>200</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="5">
         <v>4</v>
       </c>
-      <c r="B7" s="5">
-        <v>30</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="8">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="2">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>14</v>
+      <c r="C9" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="5">
+        <v>30</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="8">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B13" s="5">
         <v>1</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="C13" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B11" s="5">
-        <v>6</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B12" s="5">
-        <v>5</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="10">
-        <v>200</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="D13" s="12" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
       <c r="B14" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="B15" s="5">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="8">
-        <v>30</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>13</v>
-      </c>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="10">
+        <v>1</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16" s="6"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="2">
-        <v>3</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>14</v>
+      <c r="A17" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B17" s="5">
+        <v>6</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B18" s="5">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B19" s="5">
-        <v>8</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>9</v>
+      <c r="A19" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="10">
+        <v>200</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="5">
+        <v>6</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="5">
+        <v>20</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="8">
+        <v>30</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="2">
+        <v>3</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="5">
         <v>2</v>
       </c>
-      <c r="B20" s="5">
+      <c r="C24" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="5">
         <v>10</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D20" s="6" t="s">
+      <c r="C26" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="10">
+        <v>1</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="5">
+        <v>8</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B29" s="5">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="11" t="s">
+      <c r="C29" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B30" s="10">
         <v>200</v>
       </c>
-      <c r="C21" s="10" t="s">
+      <c r="C30" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D30" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B31" s="5">
         <v>8</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D22" s="6" t="s">
+      <c r="C31" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D31" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B32" s="5">
         <v>10</v>
       </c>
-      <c r="C23" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="C32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="6" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="7" t="s">
+    <row r="33" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="8">
+      <c r="B33" s="8">
         <v>20</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D24" s="9" t="s">
+      <c r="C33" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="9" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
boss pattern added and paramters fixed
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/boss_pattern.xlsx
+++ b/Engine/data/datasheet/boss_pattern.xlsx
@@ -1,26 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\datasheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Junsoo C\Desktop\kraftonClient\Engine\data\datasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEF23EA-A07A-4940-A69D-B88E338432A2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D324A40C-6BE3-4150-AC22-E583DA24E16C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="boss_parameter" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="25">
   <si>
     <t>int</t>
     <phoneticPr fontId="18" type="noConversion"/>
@@ -468,7 +475,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -663,6 +670,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color theme="5" tint="0.39994506668294322"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color theme="5" tint="0.39994506668294322"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color theme="5" tint="0.39994506668294322"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -792,7 +830,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -830,6 +868,15 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1187,10 +1234,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:D165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
+      <selection activeCell="B132" sqref="B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1260,7 +1307,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="10">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>24</v>
@@ -1369,8 +1416,8 @@
       <c r="A13" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B13" s="5">
-        <v>1</v>
+      <c r="B13" s="10">
+        <v>0</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>0</v>
@@ -1383,11 +1430,11 @@
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="5">
-        <v>1</v>
+      <c r="B14" s="10">
+        <v>0</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>19</v>
@@ -1397,11 +1444,11 @@
       <c r="A15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="5">
-        <v>50</v>
+      <c r="B15" s="10">
+        <v>30</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>22</v>
@@ -1412,7 +1459,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="10">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>24</v>
@@ -1423,8 +1470,8 @@
       <c r="A17" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="5">
-        <v>6</v>
+      <c r="B17" s="10">
+        <v>1</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>0</v>
@@ -1437,8 +1484,8 @@
       <c r="A18" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="5">
-        <v>5</v>
+      <c r="B18" s="10">
+        <v>0</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>0</v>
@@ -1455,7 +1502,7 @@
         <v>200</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D19" s="12" t="s">
         <v>17</v>
@@ -1465,8 +1512,8 @@
       <c r="A20" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B20" s="5">
-        <v>6</v>
+      <c r="B20" s="10">
+        <v>5</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>0</v>
@@ -1479,8 +1526,8 @@
       <c r="A21" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B21" s="5">
-        <v>20</v>
+      <c r="B21" s="10">
+        <v>40</v>
       </c>
       <c r="C21" s="5" t="s">
         <v>0</v>
@@ -1494,7 +1541,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="8">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>0</v>
@@ -1521,8 +1568,8 @@
       <c r="A24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B24" s="5">
-        <v>2</v>
+      <c r="B24" s="10">
+        <v>0</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>0</v>
@@ -1536,10 +1583,10 @@
         <v>21</v>
       </c>
       <c r="B25" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>19</v>
@@ -1549,11 +1596,11 @@
       <c r="A26" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B26" s="5">
-        <v>10</v>
+      <c r="B26" s="10">
+        <v>70</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>22</v>
@@ -1564,7 +1611,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="10">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>24</v>
@@ -1575,8 +1622,8 @@
       <c r="A28" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="5">
-        <v>8</v>
+      <c r="B28" s="10">
+        <v>5</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>0</v>
@@ -1589,7 +1636,7 @@
       <c r="A29" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="10">
         <v>10</v>
       </c>
       <c r="C29" s="5" t="s">
@@ -1607,7 +1654,7 @@
         <v>200</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="D30" s="12" t="s">
         <v>17</v>
@@ -1617,8 +1664,8 @@
       <c r="A31" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="5">
-        <v>8</v>
+      <c r="B31" s="10">
+        <v>3</v>
       </c>
       <c r="C31" s="5" t="s">
         <v>0</v>
@@ -1631,8 +1678,8 @@
       <c r="A32" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B32" s="5">
-        <v>10</v>
+      <c r="B32" s="10">
+        <v>40</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>0</v>
@@ -1646,12 +1693,1836 @@
         <v>5</v>
       </c>
       <c r="B33" s="8">
+        <v>0</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="2">
+        <v>4</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B35" s="10">
+        <v>0</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B36" s="5">
+        <v>0</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="9" t="s">
+      <c r="B37" s="10">
+        <v>80</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D38" s="6"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="10">
+        <v>9</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="10">
+        <v>40</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="10">
+        <v>200</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="10">
+        <v>3</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="10">
+        <v>40</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="8">
+        <v>-20</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B45" s="2">
+        <v>5</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="10">
+        <v>0</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="10">
+        <v>100</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" s="6"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B50" s="10">
+        <v>3</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="10">
+        <v>50</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B52" s="10">
+        <v>200</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D52" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="10">
+        <v>2</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B54" s="10">
+        <v>40</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B55" s="5">
+        <v>0</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B56" s="14">
+        <v>6</v>
+      </c>
+      <c r="C56" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B57" s="5">
+        <v>1</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B58" s="5">
+        <v>1</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B59" s="5">
+        <v>10</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B60" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B61" s="5">
+        <v>1</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="5">
+        <v>120</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B63" s="10">
+        <v>100</v>
+      </c>
+      <c r="C63" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64" s="5">
+        <v>2</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B65" s="5">
+        <v>50</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B66" s="8">
+        <v>30</v>
+      </c>
+      <c r="C66" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B67" s="2">
+        <v>7</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B68" s="5">
+        <v>1</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B69" s="10">
+        <v>0</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B70" s="10">
+        <v>120</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B71" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="C71" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D71" s="6"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="10">
+        <v>6</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="10">
+        <v>60</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B74" s="10">
+        <v>250</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="10">
+        <v>2</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B76" s="10">
+        <v>60</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A77" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B77" s="8">
+        <v>30</v>
+      </c>
+      <c r="C77" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B78" s="2">
+        <v>8</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B79" s="5">
+        <v>1</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B80" s="5">
+        <v>0</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B81" s="10">
+        <v>40</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B82" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C82" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D82" s="6"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B83" s="10">
+        <v>2</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B84" s="10">
+        <v>180</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B85" s="10">
+        <v>200</v>
+      </c>
+      <c r="C85" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D85" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86" s="10">
+        <v>20</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D86" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B87" s="10">
+        <v>20</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A88" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" s="8">
+        <v>-10</v>
+      </c>
+      <c r="C88" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D88" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B89" s="2">
+        <v>9</v>
+      </c>
+      <c r="C89" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D89" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B90" s="5">
+        <v>1</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B91" s="5">
+        <v>0</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B92" s="10">
+        <v>40</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B93" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C93" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" s="6"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B94" s="10">
+        <v>5</v>
+      </c>
+      <c r="C94" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B95" s="10">
+        <v>10</v>
+      </c>
+      <c r="C95" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B96" s="10">
+        <v>200</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D96" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B97" s="10">
+        <v>3</v>
+      </c>
+      <c r="C97" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B98" s="10">
+        <v>30</v>
+      </c>
+      <c r="C98" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B99" s="8">
+        <v>-5</v>
+      </c>
+      <c r="C99" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B100" s="2">
+        <v>10</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B101" s="5">
+        <v>1</v>
+      </c>
+      <c r="C101" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B102" s="5">
+        <v>0</v>
+      </c>
+      <c r="C102" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D102" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B103" s="10">
+        <v>10</v>
+      </c>
+      <c r="C103" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B104" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="C104" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D104" s="6"/>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B105" s="10">
+        <v>8</v>
+      </c>
+      <c r="C105" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="10">
+        <v>45</v>
+      </c>
+      <c r="C106" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B107" s="10">
+        <v>200</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B108" s="10">
+        <v>5</v>
+      </c>
+      <c r="C108" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B109" s="10">
+        <v>30</v>
+      </c>
+      <c r="C109" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A110" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B110" s="10">
+        <v>20</v>
+      </c>
+      <c r="C110" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D110" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="17.25" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A111" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B111" s="14">
+        <v>11</v>
+      </c>
+      <c r="C111" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="D111" s="15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B112" s="5">
+        <v>2</v>
+      </c>
+      <c r="C112" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B113" s="5">
+        <v>0</v>
+      </c>
+      <c r="C113" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B114" s="5">
+        <v>10</v>
+      </c>
+      <c r="C114" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D114" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B115" s="10">
+        <v>0.3</v>
+      </c>
+      <c r="C115" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D115" s="6"/>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A116" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B116" s="5">
+        <v>8</v>
+      </c>
+      <c r="C116" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A117" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B117" s="5">
+        <v>45</v>
+      </c>
+      <c r="C117" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A118" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B118" s="10">
+        <v>100</v>
+      </c>
+      <c r="C118" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D118" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A119" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B119" s="5">
+        <v>8</v>
+      </c>
+      <c r="C119" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D119" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A120" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B120" s="5">
+        <v>10</v>
+      </c>
+      <c r="C120" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A121" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B121" s="8">
+        <v>20</v>
+      </c>
+      <c r="C121" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A122" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B122" s="2">
+        <v>12</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A123" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B123" s="5">
+        <v>2</v>
+      </c>
+      <c r="C123" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D123" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A124" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B124" s="10">
+        <v>0</v>
+      </c>
+      <c r="C124" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D124" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A125" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B125" s="10">
+        <v>20</v>
+      </c>
+      <c r="C125" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D125" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A126" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B126" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="C126" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D126" s="6"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A127" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B127" s="10">
+        <v>4</v>
+      </c>
+      <c r="C127" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D127" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A128" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B128" s="10">
+        <v>90</v>
+      </c>
+      <c r="C128" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D128" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A129" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B129" s="10">
+        <v>200</v>
+      </c>
+      <c r="C129" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D129" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A130" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B130" s="10">
+        <v>30</v>
+      </c>
+      <c r="C130" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D130" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A131" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B131" s="10">
+        <v>30</v>
+      </c>
+      <c r="C131" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D131" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B132" s="8">
+        <v>-10</v>
+      </c>
+      <c r="C132" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D132" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A133" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B133" s="2">
+        <v>13</v>
+      </c>
+      <c r="C133" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A134" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B134" s="5">
+        <v>2</v>
+      </c>
+      <c r="C134" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D134" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A135" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B135" s="10">
+        <v>0</v>
+      </c>
+      <c r="C135" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D135" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A136" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B136" s="10">
+        <v>100</v>
+      </c>
+      <c r="C136" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D136" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A137" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B137" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="C137" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D137" s="6"/>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A138" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B138" s="10">
+        <v>12</v>
+      </c>
+      <c r="C138" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D138" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A139" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B139" s="10">
+        <v>30</v>
+      </c>
+      <c r="C139" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D139" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A140" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B140" s="10">
+        <v>200</v>
+      </c>
+      <c r="C140" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D140" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A141" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B141" s="10">
+        <v>5</v>
+      </c>
+      <c r="C141" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D141" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A142" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B142" s="10">
+        <v>30</v>
+      </c>
+      <c r="C142" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D142" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="143" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A143" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B143" s="8">
+        <v>5</v>
+      </c>
+      <c r="C143" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D143" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A144" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B144" s="2">
+        <v>14</v>
+      </c>
+      <c r="C144" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D144" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A145" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B145" s="5">
+        <v>2</v>
+      </c>
+      <c r="C145" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D145" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A146" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B146" s="5">
+        <v>1</v>
+      </c>
+      <c r="C146" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D146" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A147" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B147" s="10">
+        <v>20</v>
+      </c>
+      <c r="C147" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D147" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A148" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B148" s="10">
+        <v>0.7</v>
+      </c>
+      <c r="C148" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D148" s="6"/>
+    </row>
+    <row r="149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A149" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B149" s="10">
+        <v>2</v>
+      </c>
+      <c r="C149" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D149" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A150" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B150" s="10">
+        <v>200</v>
+      </c>
+      <c r="C150" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D150" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A151" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B151" s="10">
+        <v>50</v>
+      </c>
+      <c r="C151" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D151" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A152" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B152" s="10">
+        <v>1</v>
+      </c>
+      <c r="C152" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D152" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A153" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B153" s="10">
+        <v>0</v>
+      </c>
+      <c r="C153" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D153" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A154" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B154" s="8">
+        <v>0</v>
+      </c>
+      <c r="C154" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D154" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A155" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B155" s="2">
+        <v>15</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A156" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B156" s="5">
+        <v>2</v>
+      </c>
+      <c r="C156" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D156" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A157" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B157" s="5">
+        <v>0</v>
+      </c>
+      <c r="C157" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D157" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A158" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B158" s="10">
+        <v>30</v>
+      </c>
+      <c r="C158" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D158" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A159" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B159" s="10">
+        <v>0.6</v>
+      </c>
+      <c r="C159" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D159" s="6"/>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A160" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B160" s="10">
+        <v>6</v>
+      </c>
+      <c r="C160" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D160" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A161" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B161" s="10">
+        <v>60</v>
+      </c>
+      <c r="C161" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D161" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A162" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B162" s="10">
+        <v>200</v>
+      </c>
+      <c r="C162" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D162" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A163" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B163" s="10">
+        <v>6</v>
+      </c>
+      <c r="C163" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D163" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A164" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B164" s="10">
+        <v>50</v>
+      </c>
+      <c r="C164" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D164" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A165" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B165" s="8">
+        <v>30</v>
+      </c>
+      <c r="C165" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D165" s="9" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[FINAL] boss pattern frame fixed
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/boss_pattern.xlsx
+++ b/Engine/data/datasheet/boss_pattern.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Junsoo C\Desktop\kraftonClient\Engine\data\datasheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\datasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D324A40C-6BE3-4150-AC22-E583DA24E16C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972EDF8E-EED5-4C6D-859F-125247543CDE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="boss_parameter" sheetId="1" r:id="rId1"/>
@@ -1236,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" workbookViewId="0">
-      <selection activeCell="B132" sqref="B132"/>
+    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="C120" sqref="C120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1307,7 +1307,7 @@
         <v>23</v>
       </c>
       <c r="B5" s="10">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>24</v>
@@ -1459,7 +1459,7 @@
         <v>23</v>
       </c>
       <c r="B16" s="10">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>24</v>
@@ -1611,7 +1611,7 @@
         <v>23</v>
       </c>
       <c r="B27" s="10">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>24</v>
@@ -1763,7 +1763,7 @@
         <v>23</v>
       </c>
       <c r="B38" s="10">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="C38" s="10" t="s">
         <v>24</v>
@@ -1915,7 +1915,7 @@
         <v>23</v>
       </c>
       <c r="B49" s="10">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>24</v>
@@ -2053,7 +2053,7 @@
         <v>20</v>
       </c>
       <c r="B59" s="5">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>0</v>
@@ -2067,7 +2067,7 @@
         <v>23</v>
       </c>
       <c r="B60" s="10">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="C60" s="10" t="s">
         <v>24</v>
@@ -2107,7 +2107,7 @@
         <v>15</v>
       </c>
       <c r="B63" s="10">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>0</v>
@@ -2135,7 +2135,7 @@
         <v>4</v>
       </c>
       <c r="B65" s="5">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C65" s="5" t="s">
         <v>0</v>
@@ -2219,7 +2219,7 @@
         <v>23</v>
       </c>
       <c r="B71" s="10">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>24</v>
@@ -2371,7 +2371,7 @@
         <v>23</v>
       </c>
       <c r="B82" s="10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>24</v>
@@ -2523,7 +2523,7 @@
         <v>23</v>
       </c>
       <c r="B93" s="10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>24</v>
@@ -2675,7 +2675,7 @@
         <v>23</v>
       </c>
       <c r="B104" s="10">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>24</v>
@@ -2867,7 +2867,7 @@
         <v>15</v>
       </c>
       <c r="B118" s="10">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="C118" s="10" t="s">
         <v>0</v>
@@ -2881,7 +2881,7 @@
         <v>3</v>
       </c>
       <c r="B119" s="5">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>0</v>
@@ -2979,7 +2979,7 @@
         <v>23</v>
       </c>
       <c r="B126" s="10">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C126" s="10" t="s">
         <v>24</v>
@@ -2991,7 +2991,7 @@
         <v>1</v>
       </c>
       <c r="B127" s="10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C127" s="5" t="s">
         <v>0</v>
@@ -3019,7 +3019,7 @@
         <v>15</v>
       </c>
       <c r="B129" s="10">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C129" s="10" t="s">
         <v>0</v>
@@ -3131,7 +3131,7 @@
         <v>23</v>
       </c>
       <c r="B137" s="10">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="C137" s="10" t="s">
         <v>24</v>
@@ -3171,7 +3171,7 @@
         <v>15</v>
       </c>
       <c r="B140" s="10">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="C140" s="10" t="s">
         <v>0</v>
@@ -3185,7 +3185,7 @@
         <v>3</v>
       </c>
       <c r="B141" s="10">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C141" s="5" t="s">
         <v>0</v>
@@ -3269,7 +3269,7 @@
         <v>20</v>
       </c>
       <c r="B147" s="10">
-        <v>20</v>
+        <v>300</v>
       </c>
       <c r="C147" s="5" t="s">
         <v>0</v>
@@ -3283,7 +3283,7 @@
         <v>23</v>
       </c>
       <c r="B148" s="10">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="C148" s="10" t="s">
         <v>24</v>
@@ -3295,7 +3295,7 @@
         <v>1</v>
       </c>
       <c r="B149" s="10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C149" s="5" t="s">
         <v>0</v>
@@ -3309,7 +3309,7 @@
         <v>2</v>
       </c>
       <c r="B150" s="10">
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="C150" s="5" t="s">
         <v>0</v>
@@ -3323,7 +3323,7 @@
         <v>15</v>
       </c>
       <c r="B151" s="10">
-        <v>50</v>
+        <v>500</v>
       </c>
       <c r="C151" s="10" t="s">
         <v>0</v>
@@ -3435,7 +3435,7 @@
         <v>23</v>
       </c>
       <c r="B159" s="10">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="C159" s="10" t="s">
         <v>24</v>
@@ -3475,7 +3475,7 @@
         <v>15</v>
       </c>
       <c r="B162" s="10">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="C162" s="10" t="s">
         <v>0</v>
@@ -3489,7 +3489,7 @@
         <v>3</v>
       </c>
       <c r="B163" s="10">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C163" s="5" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
bullet delete and balancing
</commit_message>
<xml_diff>
--- a/Engine/data/datasheet/boss_pattern.xlsx
+++ b/Engine/data/datasheet/boss_pattern.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\js_choi\Desktop\mainproject\Engine\Engine\data\datasheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972EDF8E-EED5-4C6D-859F-125247543CDE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12A72219-7566-4359-B243-8D9A511FEA57}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1236,8 +1236,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="C120" sqref="C120"/>
+    <sheetView tabSelected="1" topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="D117" sqref="D117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2053,7 +2053,7 @@
         <v>20</v>
       </c>
       <c r="B59" s="5">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>0</v>
@@ -2107,7 +2107,7 @@
         <v>15</v>
       </c>
       <c r="B63" s="10">
-        <v>200</v>
+        <v>700</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>0</v>
@@ -2881,7 +2881,7 @@
         <v>3</v>
       </c>
       <c r="B119" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>0</v>
@@ -3143,7 +3143,7 @@
         <v>1</v>
       </c>
       <c r="B138" s="10">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C138" s="5" t="s">
         <v>0</v>
@@ -3157,7 +3157,7 @@
         <v>2</v>
       </c>
       <c r="B139" s="10">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C139" s="5" t="s">
         <v>0</v>
@@ -3323,7 +3323,7 @@
         <v>15</v>
       </c>
       <c r="B151" s="10">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="C151" s="10" t="s">
         <v>0</v>
@@ -3489,7 +3489,7 @@
         <v>3</v>
       </c>
       <c r="B163" s="10">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C163" s="5" t="s">
         <v>0</v>

</xml_diff>